<commit_message>
data updated for new items
</commit_message>
<xml_diff>
--- a/Code/vajrang/September2022/Data/input.xlsx
+++ b/Code/vajrang/September2022/Data/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\Code\vajrang\September2022\Week3\LogItems\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\Code\vajrang\September2022\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045AD104-2FC9-4013-AEAA-CD34FAA49E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45381498-596B-4E9C-B848-59008669366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="2565" windowWidth="16200" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1485" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>Items</t>
   </si>
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,6 +390,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>